<commit_message>
add custom tarifas ranges
</commit_message>
<xml_diff>
--- a/assets/downloads/Boleta_Template.xlsx
+++ b/assets/downloads/Boleta_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\probusinees-intranet\assets\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831B021A-28F5-4906-9311-4CD9EC766461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EEDC7A5-C734-4A06-B939-4224713D8E36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1257,6 +1257,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1270,18 +1279,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="7" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="7" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="172" fontId="7" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1323,11 +1320,14 @@
     <xf numFmtId="14" fontId="8" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="7" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="172" fontId="7" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2174,50 +2174,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>970642</xdr:colOff>
-      <xdr:row>94</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>439808</xdr:colOff>
-      <xdr:row>108</xdr:row>
-      <xdr:rowOff>195956</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Imagen 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2367642" y="19554825"/>
-          <a:ext cx="3761670" cy="2796281"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
@@ -2305,6 +2261,50 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>414152</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>180107</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>352926</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>177579</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70D6B73D-ECE3-0CF5-9019-607B3F36EC7C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1841170" y="17609125"/>
+          <a:ext cx="4289101" cy="3280999"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -2576,8 +2576,8 @@
   <sheetPr codeName="Hoja2"/>
   <dimension ref="B1:L109"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36:L41"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A83" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="M115" sqref="M115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="14.4"/>
@@ -2609,16 +2609,16 @@
       <c r="L2" s="29"/>
     </row>
     <row r="3" spans="2:12">
-      <c r="G3" s="110"/>
-      <c r="H3" s="110"/>
-      <c r="I3" s="110"/>
-      <c r="J3" s="110"/>
+      <c r="G3" s="109"/>
+      <c r="H3" s="109"/>
+      <c r="I3" s="109"/>
+      <c r="J3" s="109"/>
     </row>
     <row r="4" spans="2:12">
-      <c r="G4" s="111"/>
-      <c r="H4" s="111"/>
-      <c r="I4" s="111"/>
-      <c r="J4" s="111"/>
+      <c r="G4" s="110"/>
+      <c r="H4" s="110"/>
+      <c r="I4" s="110"/>
+      <c r="J4" s="110"/>
       <c r="K4" s="38"/>
     </row>
     <row r="6" spans="2:12">
@@ -2629,11 +2629,11 @@
       <c r="H6" s="64"/>
     </row>
     <row r="7" spans="2:12">
-      <c r="E7" s="117" t="s">
+      <c r="E7" s="116" t="s">
         <v>121</v>
       </c>
-      <c r="F7" s="117"/>
-      <c r="G7" s="117"/>
+      <c r="F7" s="116"/>
+      <c r="G7" s="116"/>
     </row>
     <row r="8" spans="2:12">
       <c r="B8" s="31" t="s">
@@ -2653,12 +2653,12 @@
       <c r="I8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="J8" s="115">
+      <c r="J8" s="114">
         <f>+'2'!F7</f>
         <v>8</v>
       </c>
-      <c r="K8" s="115"/>
-      <c r="L8" s="115"/>
+      <c r="K8" s="114"/>
+      <c r="L8" s="114"/>
     </row>
     <row r="9" spans="2:12">
       <c r="B9" s="31" t="s">
@@ -2670,21 +2670,21 @@
       <c r="E9" s="61" t="s">
         <v>104</v>
       </c>
-      <c r="F9" s="121">
+      <c r="F9" s="120">
         <f ca="1">+TODAY()</f>
-        <v>45439</v>
-      </c>
-      <c r="G9" s="122"/>
+        <v>45455</v>
+      </c>
+      <c r="G9" s="121"/>
       <c r="H9" s="29"/>
       <c r="I9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J9" s="116">
+      <c r="J9" s="115">
         <f>+'2'!F8</f>
         <v>116</v>
       </c>
-      <c r="K9" s="116"/>
-      <c r="L9" s="116"/>
+      <c r="K9" s="115"/>
+      <c r="L9" s="115"/>
     </row>
     <row r="10" spans="2:12">
       <c r="B10" s="31" t="s">
@@ -2729,21 +2729,21 @@
       <c r="I11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="119">
+      <c r="J11" s="118">
         <f>+'2'!F9</f>
         <v>1.1879999999999999</v>
       </c>
-      <c r="K11" s="119"/>
-      <c r="L11" s="119"/>
+      <c r="K11" s="118"/>
+      <c r="L11" s="118"/>
     </row>
     <row r="13" spans="2:12">
-      <c r="B13" s="118" t="s">
+      <c r="B13" s="117" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="118"/>
-      <c r="D13" s="118"/>
-      <c r="E13" s="118"/>
-      <c r="F13" s="118"/>
+      <c r="C13" s="117"/>
+      <c r="D13" s="117"/>
+      <c r="E13" s="117"/>
+      <c r="F13" s="117"/>
       <c r="G13" s="52"/>
       <c r="H13" s="52"/>
       <c r="I13" s="54"/>
@@ -2756,11 +2756,11 @@
       </c>
     </row>
     <row r="14" spans="2:12">
-      <c r="B14" s="124" t="s">
+      <c r="B14" s="103" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="124"/>
-      <c r="D14" s="124"/>
+      <c r="C14" s="103"/>
+      <c r="D14" s="103"/>
       <c r="E14" s="29"/>
       <c r="F14" s="29"/>
       <c r="G14" s="29"/>
@@ -2774,11 +2774,11 @@
       </c>
     </row>
     <row r="15" spans="2:12">
-      <c r="B15" s="123" t="s">
+      <c r="B15" s="102" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="123"/>
-      <c r="D15" s="123"/>
+      <c r="C15" s="102"/>
+      <c r="D15" s="102"/>
       <c r="E15" s="36"/>
       <c r="F15" s="36"/>
       <c r="G15" s="36"/>
@@ -2840,13 +2840,13 @@
       <c r="L18" s="29"/>
     </row>
     <row r="19" spans="2:12">
-      <c r="B19" s="118" t="s">
+      <c r="B19" s="117" t="s">
         <v>102</v>
       </c>
-      <c r="C19" s="118"/>
-      <c r="D19" s="118"/>
-      <c r="E19" s="118"/>
-      <c r="F19" s="118"/>
+      <c r="C19" s="117"/>
+      <c r="D19" s="117"/>
+      <c r="E19" s="117"/>
+      <c r="F19" s="117"/>
       <c r="G19" s="52"/>
       <c r="H19" s="52"/>
       <c r="I19" s="52"/>
@@ -3002,13 +3002,13 @@
       </c>
     </row>
     <row r="28" spans="2:12" ht="15.6">
-      <c r="B28" s="120" t="s">
+      <c r="B28" s="119" t="s">
         <v>99</v>
       </c>
-      <c r="C28" s="120"/>
-      <c r="D28" s="120"/>
-      <c r="E28" s="120"/>
-      <c r="F28" s="120"/>
+      <c r="C28" s="119"/>
+      <c r="D28" s="119"/>
+      <c r="E28" s="119"/>
+      <c r="F28" s="119"/>
       <c r="G28" s="72"/>
       <c r="H28" s="72"/>
       <c r="I28" s="73"/>
@@ -3114,66 +3114,66 @@
       <c r="L33" s="32"/>
     </row>
     <row r="34" spans="2:12">
-      <c r="B34" s="112" t="s">
+      <c r="B34" s="111" t="s">
         <v>103</v>
       </c>
-      <c r="C34" s="113"/>
-      <c r="D34" s="113"/>
-      <c r="E34" s="113"/>
-      <c r="F34" s="113"/>
-      <c r="G34" s="113"/>
-      <c r="H34" s="113"/>
-      <c r="I34" s="113"/>
-      <c r="J34" s="113"/>
-      <c r="K34" s="113"/>
-      <c r="L34" s="114"/>
+      <c r="C34" s="112"/>
+      <c r="D34" s="112"/>
+      <c r="E34" s="112"/>
+      <c r="F34" s="112"/>
+      <c r="G34" s="112"/>
+      <c r="H34" s="112"/>
+      <c r="I34" s="112"/>
+      <c r="J34" s="112"/>
+      <c r="K34" s="112"/>
+      <c r="L34" s="113"/>
     </row>
     <row r="35" spans="2:12">
       <c r="B35" s="53" t="s">
         <v>45</v>
       </c>
-      <c r="C35" s="101" t="s">
+      <c r="C35" s="104" t="s">
         <v>80</v>
       </c>
-      <c r="D35" s="102"/>
-      <c r="E35" s="103"/>
+      <c r="D35" s="105"/>
+      <c r="E35" s="106"/>
       <c r="F35" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G35" s="101" t="s">
+      <c r="G35" s="104" t="s">
         <v>81</v>
       </c>
-      <c r="H35" s="103"/>
+      <c r="H35" s="106"/>
       <c r="I35" s="5" t="s">
         <v>78</v>
       </c>
       <c r="J35" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="K35" s="107" t="s">
+      <c r="K35" s="101" t="s">
         <v>79</v>
       </c>
-      <c r="L35" s="107"/>
+      <c r="L35" s="101"/>
     </row>
     <row r="36" spans="2:12">
       <c r="B36" s="53">
         <v>1</v>
       </c>
-      <c r="C36" s="101" t="str">
+      <c r="C36" s="104" t="str">
         <f>+'2'!$C$6</f>
         <v xml:space="preserve">Kids Car Seat Belt Pillow </v>
       </c>
-      <c r="D36" s="102"/>
-      <c r="E36" s="103"/>
+      <c r="D36" s="105"/>
+      <c r="E36" s="106"/>
       <c r="F36" s="7">
         <f>+'2'!$C$45</f>
         <v>100</v>
       </c>
-      <c r="G36" s="104">
+      <c r="G36" s="107">
         <f>+'2'!$C$10</f>
         <v>6.36</v>
       </c>
-      <c r="H36" s="105"/>
+      <c r="H36" s="108"/>
       <c r="I36" s="66">
         <f>+'2'!$C$46</f>
         <v>11.424505892807643</v>
@@ -3182,31 +3182,31 @@
         <f t="shared" ref="J36:J38" si="0">+F36*I36</f>
         <v>1142.4505892807642</v>
       </c>
-      <c r="K36" s="107">
+      <c r="K36" s="101">
         <f t="shared" ref="K36" si="1">I36*3.7</f>
         <v>42.270671803388282</v>
       </c>
-      <c r="L36" s="107"/>
+      <c r="L36" s="101"/>
     </row>
     <row r="37" spans="2:12">
       <c r="B37" s="53">
         <v>2</v>
       </c>
-      <c r="C37" s="101" t="str">
+      <c r="C37" s="104" t="str">
         <f>+'2'!$D$6</f>
         <v>Car Headrest</v>
       </c>
-      <c r="D37" s="102"/>
-      <c r="E37" s="103"/>
+      <c r="D37" s="105"/>
+      <c r="E37" s="106"/>
       <c r="F37" s="7">
         <f>+'2'!$D$45</f>
         <v>1</v>
       </c>
-      <c r="G37" s="104">
+      <c r="G37" s="107">
         <f>+'2'!$D$10</f>
         <v>8.0299999999999994</v>
       </c>
-      <c r="H37" s="105"/>
+      <c r="H37" s="108"/>
       <c r="I37" s="66">
         <f>+'2'!$D$46</f>
         <v>13.907609574791055</v>
@@ -3215,31 +3215,31 @@
         <f t="shared" si="0"/>
         <v>13.907609574791055</v>
       </c>
-      <c r="K37" s="107">
+      <c r="K37" s="101">
         <f t="shared" ref="K37:K38" si="2">I37*3.7</f>
         <v>51.458155426726904</v>
       </c>
-      <c r="L37" s="107"/>
+      <c r="L37" s="101"/>
     </row>
     <row r="38" spans="2:12">
       <c r="B38" s="53">
         <v>3</v>
       </c>
-      <c r="C38" s="101" t="str">
+      <c r="C38" s="104" t="str">
         <f>+'2'!$E$6</f>
         <v>Bluetooth sleep mask</v>
       </c>
-      <c r="D38" s="102"/>
-      <c r="E38" s="103"/>
+      <c r="D38" s="105"/>
+      <c r="E38" s="106"/>
       <c r="F38" s="7">
         <f>+'2'!$E$45</f>
         <v>50</v>
       </c>
-      <c r="G38" s="104">
+      <c r="G38" s="107">
         <f>+'2'!$E$10</f>
         <v>6</v>
       </c>
-      <c r="H38" s="105"/>
+      <c r="H38" s="108"/>
       <c r="I38" s="66">
         <f>+'2'!$E$46</f>
         <v>10.391738162982108</v>
@@ -3248,11 +3248,11 @@
         <f t="shared" si="0"/>
         <v>519.5869081491054</v>
       </c>
-      <c r="K38" s="108">
+      <c r="K38" s="123">
         <f t="shared" si="2"/>
         <v>38.449431203033804</v>
       </c>
-      <c r="L38" s="109"/>
+      <c r="L38" s="124"/>
     </row>
     <row r="39" spans="2:12" ht="15.6">
       <c r="B39" s="57" t="s">
@@ -3413,19 +3413,19 @@
       <c r="K53" s="38"/>
     </row>
     <row r="55" spans="2:12" ht="21">
-      <c r="B55" s="106" t="s">
+      <c r="B55" s="122" t="s">
         <v>44</v>
       </c>
-      <c r="C55" s="106"/>
-      <c r="D55" s="106"/>
-      <c r="E55" s="106"/>
-      <c r="F55" s="106"/>
-      <c r="G55" s="106"/>
-      <c r="H55" s="106"/>
-      <c r="I55" s="106"/>
-      <c r="J55" s="106"/>
-      <c r="K55" s="106"/>
-      <c r="L55" s="106"/>
+      <c r="C55" s="122"/>
+      <c r="D55" s="122"/>
+      <c r="E55" s="122"/>
+      <c r="F55" s="122"/>
+      <c r="G55" s="122"/>
+      <c r="H55" s="122"/>
+      <c r="I55" s="122"/>
+      <c r="J55" s="122"/>
+      <c r="K55" s="122"/>
+      <c r="L55" s="122"/>
     </row>
     <row r="59" spans="2:12">
       <c r="B59" s="46" t="s">
@@ -3746,11 +3746,13 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="26">
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="B55:L55"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="K38:L38"/>
     <mergeCell ref="G3:J3"/>
     <mergeCell ref="G4:J4"/>
     <mergeCell ref="G35:H35"/>
@@ -3765,13 +3767,11 @@
     <mergeCell ref="J11:L11"/>
     <mergeCell ref="B28:F28"/>
     <mergeCell ref="F9:G9"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="B55:L55"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="K38:L38"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="G36:H36"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="VERIFICAR NÚMERO DE TELEFONO" error="Verifica que tenga 9 digitos sin espacio" sqref="J8:L8" xr:uid="{CC0405B2-A74A-4E8F-BF03-C34BEE695B67}">

</xml_diff>